<commit_message>
update Bordeaux neighborhood database
</commit_message>
<xml_diff>
--- a/Quartiers_Bordeaux.xlsx
+++ b/Quartiers_Bordeaux.xlsx
@@ -64,7 +64,7 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Lattitude</t>
+    <t>Latitude</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="B1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,10 +428,10 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>